<commit_message>
Chaning CSS and add view 3 file
</commit_message>
<xml_diff>
--- a/Requirement/Profile General Requirement.xlsx
+++ b/Requirement/Profile General Requirement.xlsx
@@ -833,10 +833,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -845,17 +848,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5491,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BT188"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="O101" sqref="O101"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A64" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5506,30 +5506,30 @@
       <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="48"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="46"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -5537,135 +5537,135 @@
       <c r="C6" s="12">
         <v>2</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46" t="s">
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="46"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="12">
         <v>3</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49" t="s">
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="49"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C8" s="12">
         <v>4</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49" t="s">
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="49"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9" s="12">
         <v>5</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46" t="s">
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="46"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10" s="12">
         <v>6</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="44" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="45"/>
+      <c r="H10" s="46"/>
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" s="12">
         <v>7</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="44" t="s">
+      <c r="E11" s="48"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="45"/>
+      <c r="H11" s="46"/>
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C12" s="12">
         <v>8</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46" t="s">
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="46"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13" s="12">
         <v>9</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46" t="s">
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="46"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="11"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="12">
         <v>10</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="46"/>
+      <c r="H14" s="43"/>
       <c r="I14" s="11"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -8394,11 +8394,11 @@
     <row r="83" spans="1:55" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="25"/>
       <c r="B83" s="29"/>
-      <c r="C83" s="43" t="s">
+      <c r="C83" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
       <c r="F83" s="29"/>
       <c r="G83" s="29"/>
       <c r="H83" s="29"/>
@@ -8528,11 +8528,11 @@
       <c r="N85" s="25"/>
       <c r="O85" s="25"/>
       <c r="P85" s="37"/>
-      <c r="Q85" s="43" t="s">
+      <c r="Q85" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="R85" s="43"/>
-      <c r="S85" s="43"/>
+      <c r="R85" s="47"/>
+      <c r="S85" s="47"/>
       <c r="T85" s="37"/>
       <c r="U85" s="37"/>
       <c r="V85" s="37"/>
@@ -8544,11 +8544,11 @@
       <c r="AB85" s="25"/>
       <c r="AC85" s="25"/>
       <c r="AD85" s="37"/>
-      <c r="AE85" s="43" t="s">
+      <c r="AE85" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="AF85" s="43"/>
-      <c r="AG85" s="43"/>
+      <c r="AF85" s="47"/>
+      <c r="AG85" s="47"/>
       <c r="AH85" s="37"/>
       <c r="AI85" s="37"/>
       <c r="AJ85" s="37"/>
@@ -8850,10 +8850,10 @@
       <c r="AE90" s="36"/>
       <c r="AF90" s="36"/>
       <c r="AG90" s="36"/>
-      <c r="AH90" s="42"/>
-      <c r="AI90" s="42"/>
-      <c r="AJ90" s="42"/>
-      <c r="AK90" s="42"/>
+      <c r="AH90" s="49"/>
+      <c r="AI90" s="49"/>
+      <c r="AJ90" s="49"/>
+      <c r="AK90" s="49"/>
       <c r="AL90" s="36"/>
       <c r="AM90" s="36"/>
       <c r="AN90" s="36"/>
@@ -8917,10 +8917,10 @@
       <c r="AE91" s="36"/>
       <c r="AF91" s="36"/>
       <c r="AG91" s="36"/>
-      <c r="AH91" s="42"/>
-      <c r="AI91" s="42"/>
-      <c r="AJ91" s="42"/>
-      <c r="AK91" s="42"/>
+      <c r="AH91" s="49"/>
+      <c r="AI91" s="49"/>
+      <c r="AJ91" s="49"/>
+      <c r="AK91" s="49"/>
       <c r="AL91" s="36"/>
       <c r="AM91" s="36"/>
       <c r="AN91" s="36"/>
@@ -10623,11 +10623,11 @@
       <c r="A121" s="25"/>
       <c r="B121" s="25"/>
       <c r="C121" s="37"/>
-      <c r="D121" s="43" t="s">
+      <c r="D121" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E121" s="43"/>
-      <c r="F121" s="43"/>
+      <c r="E121" s="47"/>
+      <c r="F121" s="47"/>
       <c r="G121" s="37"/>
       <c r="H121" s="37"/>
       <c r="I121" s="37"/>
@@ -10642,11 +10642,11 @@
       <c r="R121" s="25"/>
       <c r="S121" s="25"/>
       <c r="T121" s="37"/>
-      <c r="U121" s="43" t="s">
+      <c r="U121" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="V121" s="43"/>
-      <c r="W121" s="43"/>
+      <c r="V121" s="47"/>
+      <c r="W121" s="47"/>
       <c r="X121" s="37"/>
       <c r="Y121" s="37"/>
       <c r="Z121" s="37"/>
@@ -10915,10 +10915,10 @@
       <c r="D126" s="36"/>
       <c r="E126" s="36"/>
       <c r="F126" s="36"/>
-      <c r="G126" s="42"/>
-      <c r="H126" s="42"/>
-      <c r="I126" s="42"/>
-      <c r="J126" s="42"/>
+      <c r="G126" s="49"/>
+      <c r="H126" s="49"/>
+      <c r="I126" s="49"/>
+      <c r="J126" s="49"/>
       <c r="K126" s="36"/>
       <c r="L126" s="36"/>
       <c r="M126" s="36"/>
@@ -10932,10 +10932,10 @@
       <c r="U126" s="36"/>
       <c r="V126" s="36"/>
       <c r="W126" s="36"/>
-      <c r="X126" s="42"/>
-      <c r="Y126" s="42"/>
-      <c r="Z126" s="42"/>
-      <c r="AA126" s="42"/>
+      <c r="X126" s="49"/>
+      <c r="Y126" s="49"/>
+      <c r="Z126" s="49"/>
+      <c r="AA126" s="49"/>
       <c r="AB126" s="36"/>
       <c r="AC126" s="36"/>
       <c r="AD126" s="36"/>
@@ -10972,10 +10972,10 @@
       <c r="D127" s="36"/>
       <c r="E127" s="36"/>
       <c r="F127" s="36"/>
-      <c r="G127" s="42"/>
-      <c r="H127" s="42"/>
-      <c r="I127" s="42"/>
-      <c r="J127" s="42"/>
+      <c r="G127" s="49"/>
+      <c r="H127" s="49"/>
+      <c r="I127" s="49"/>
+      <c r="J127" s="49"/>
       <c r="K127" s="36"/>
       <c r="L127" s="36"/>
       <c r="M127" s="36"/>
@@ -10989,10 +10989,10 @@
       <c r="U127" s="36"/>
       <c r="V127" s="36"/>
       <c r="W127" s="36"/>
-      <c r="X127" s="42"/>
-      <c r="Y127" s="42"/>
-      <c r="Z127" s="42"/>
-      <c r="AA127" s="42"/>
+      <c r="X127" s="49"/>
+      <c r="Y127" s="49"/>
+      <c r="Z127" s="49"/>
+      <c r="AA127" s="49"/>
       <c r="AB127" s="36"/>
       <c r="AC127" s="36"/>
       <c r="AD127" s="36"/>
@@ -14856,16 +14856,19 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="X126:AA127"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="G126:J127"/>
+    <mergeCell ref="AE85:AG85"/>
+    <mergeCell ref="AH90:AK91"/>
+    <mergeCell ref="U121:W121"/>
+    <mergeCell ref="Q91:R92"/>
+    <mergeCell ref="S91:W92"/>
+    <mergeCell ref="X91:Z92"/>
+    <mergeCell ref="Q93:R94"/>
+    <mergeCell ref="Q95:R96"/>
+    <mergeCell ref="S93:W94"/>
+    <mergeCell ref="S95:W96"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="C83:E83"/>
@@ -14880,19 +14883,16 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="X126:AA127"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="G126:J127"/>
-    <mergeCell ref="AE85:AG85"/>
-    <mergeCell ref="AH90:AK91"/>
-    <mergeCell ref="U121:W121"/>
-    <mergeCell ref="Q91:R92"/>
-    <mergeCell ref="S91:W92"/>
-    <mergeCell ref="X91:Z92"/>
-    <mergeCell ref="Q93:R94"/>
-    <mergeCell ref="Q95:R96"/>
-    <mergeCell ref="S93:W94"/>
-    <mergeCell ref="S95:W96"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F93" r:id="rId1"/>

</xml_diff>